<commit_message>
Add Change Request Document and update Change Log
</commit_message>
<xml_diff>
--- a/docs/Change_Log.xlsx
+++ b/docs/Change_Log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apoes\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8A17F9A-411F-4FFA-B75E-54F9271DA94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACAC93C6-9417-4689-A8FD-215B6553BBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4FB8089C-7849-4B4E-8C44-7FA5D5AFABCF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>CR ID</t>
   </si>
@@ -63,21 +63,12 @@
     <t>CR-001</t>
   </si>
   <si>
-    <t>Add basic login validation</t>
-  </si>
-  <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>login.html, app.js</t>
   </si>
   <si>
     <t>High</t>
   </si>
   <si>
-    <t>Planned</t>
-  </si>
-  <si>
     <t>SCM Manager</t>
   </si>
   <si>
@@ -96,13 +87,22 @@
     <t>CR-003</t>
   </si>
   <si>
-    <t>Standardize CI naming</t>
-  </si>
-  <si>
     <t>Documentation CIs</t>
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Add login validation</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>v1.1</t>
+  </si>
+  <si>
+    <t>CI naming consistency</t>
   </si>
 </sst>
 </file>
@@ -146,12 +146,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -471,19 +474,20 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="10.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.21875" customWidth="1"/>
     <col min="7" max="7" width="15.44140625" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,82 +513,82 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="3">
+        <v>46020</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="C3" s="3">
+        <v>46020</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>10</v>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>46020</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>